<commit_message>
Added data for lean mass at sacrifice
</commit_message>
<xml_diff>
--- a/data/raw/HFD Dex Muscle Testing Data.xlsx
+++ b/data/raw/HFD Dex Muscle Testing Data.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10914"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davebrid/Documents/GitHub/CushingAcromegalyStudy/data/raw/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF087347-BEE5-744B-8568-E08DB581F707}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="0" windowWidth="21020" windowHeight="14440" tabRatio="500"/>
+    <workbookView xWindow="3600" yWindow="460" windowWidth="21020" windowHeight="14200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="19">
   <si>
     <t>Mouse ID</t>
   </si>
@@ -74,12 +80,15 @@
   <si>
     <t>Fasting Blood Glucose (mg/dL)</t>
   </si>
+  <si>
+    <t>Lean.Mass</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -119,6 +128,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -146,7 +161,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -159,6 +174,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -171,6 +187,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -495,16 +519,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" ht="60">
+    <row r="1" spans="1:14" s="3" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -544,8 +568,11 @@
       <c r="M1" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>6187</v>
       </c>
@@ -586,7 +613,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>6010</v>
       </c>
@@ -626,8 +653,11 @@
       <c r="M3" s="1">
         <v>142</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" s="7" customFormat="1">
+      <c r="N3" s="8">
+        <v>24120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="7" customFormat="1" ht="20" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>6011</v>
       </c>
@@ -667,8 +697,11 @@
       <c r="M4" s="7">
         <v>267</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="N4" s="8">
+        <v>24110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>6009</v>
       </c>
@@ -708,8 +741,11 @@
       <c r="M5" s="1">
         <v>422</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="N5" s="8">
+        <v>24800</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>6012</v>
       </c>
@@ -749,8 +785,11 @@
       <c r="M6" s="1">
         <v>154</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="N6" s="8">
+        <v>23210</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6008</v>
       </c>
@@ -790,8 +829,11 @@
       <c r="M7" s="1">
         <v>139</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="N7" s="8">
+        <v>27170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6015</v>
       </c>
@@ -831,8 +873,11 @@
       <c r="M8" s="1">
         <v>135</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="N8" s="8">
+        <v>27780</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>6014</v>
       </c>
@@ -872,8 +917,11 @@
       <c r="M9" s="1">
         <v>154</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" s="7" customFormat="1">
+      <c r="N9" s="8">
+        <v>26930</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="7" customFormat="1" ht="20" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>6013</v>
       </c>
@@ -913,8 +961,11 @@
       <c r="M10" s="7">
         <v>111</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="N10" s="8">
+        <v>28680</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>6002</v>
       </c>
@@ -954,8 +1005,11 @@
       <c r="M11" s="1">
         <v>131</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="N11" s="8">
+        <v>24700</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>6007</v>
       </c>
@@ -995,8 +1049,11 @@
       <c r="M12" s="1">
         <v>104</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="N12" s="8">
+        <v>23240</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>6003</v>
       </c>
@@ -1036,8 +1093,11 @@
       <c r="M13" s="1">
         <v>131</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="N13" s="8">
+        <v>26080</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>6000</v>
       </c>
@@ -1077,8 +1137,11 @@
       <c r="M14" s="1">
         <v>123</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="N14" s="8">
+        <v>25960</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>7125</v>
       </c>
@@ -1120,7 +1183,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>7181</v>
       </c>
@@ -1161,8 +1224,11 @@
       <c r="M16" s="1">
         <v>156</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="N16" s="8">
+        <v>25310</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>7183</v>
       </c>
@@ -1203,8 +1269,11 @@
       <c r="M17" s="1">
         <v>127</v>
       </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="N17" s="8">
+        <v>23520</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>7187</v>
       </c>
@@ -1245,8 +1314,11 @@
       <c r="M18" s="1">
         <v>184</v>
       </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="N18" s="8">
+        <v>27450</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>7186</v>
       </c>
@@ -1287,8 +1359,11 @@
       <c r="M19" s="1">
         <v>121</v>
       </c>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="N19" s="8">
+        <v>26090</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>7180</v>
       </c>
@@ -1329,8 +1404,11 @@
       <c r="M20" s="1">
         <v>143</v>
       </c>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="N20" s="8">
+        <v>20560</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>7179</v>
       </c>
@@ -1371,8 +1449,11 @@
       <c r="M21" s="1">
         <v>206</v>
       </c>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="N21" s="8">
+        <v>28280</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>7178</v>
       </c>
@@ -1413,8 +1494,11 @@
       <c r="M22" s="1">
         <v>201</v>
       </c>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="N22" s="8">
+        <v>23310</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>7185</v>
       </c>
@@ -1455,8 +1539,11 @@
       <c r="M23" s="1">
         <v>360</v>
       </c>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="N23" s="8">
+        <v>23170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>7189</v>
       </c>
@@ -1497,8 +1584,11 @@
       <c r="M24" s="1">
         <v>193</v>
       </c>
-    </row>
-    <row r="25" spans="1:13">
+      <c r="N24" s="8">
+        <v>29530</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>7176</v>
       </c>
@@ -1539,8 +1629,11 @@
       <c r="M25" s="1">
         <v>159</v>
       </c>
-    </row>
-    <row r="26" spans="1:13">
+      <c r="N25" s="8">
+        <v>23340</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>7184</v>
       </c>
@@ -1581,8 +1674,11 @@
       <c r="M26" s="1">
         <v>128</v>
       </c>
-    </row>
-    <row r="27" spans="1:13">
+      <c r="N26" s="8">
+        <v>25940</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>7188</v>
       </c>
@@ -1623,8 +1719,11 @@
       <c r="M27" s="1">
         <v>192</v>
       </c>
-    </row>
-    <row r="28" spans="1:13">
+      <c r="N27" s="8">
+        <v>29420</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>7177</v>
       </c>
@@ -1665,8 +1764,11 @@
       <c r="M28" s="1">
         <v>135</v>
       </c>
-    </row>
-    <row r="29" spans="1:13">
+      <c r="N28" s="8">
+        <v>23160</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>7182</v>
       </c>
@@ -1706,6 +1808,9 @@
       </c>
       <c r="M29" s="1">
         <v>149</v>
+      </c>
+      <c r="N29" s="8">
+        <v>24760</v>
       </c>
     </row>
   </sheetData>

</xml_diff>